<commit_message>
improved the footer and analysis tab
</commit_message>
<xml_diff>
--- a/data-raw/FIMA_APP.xlsx
+++ b/data-raw/FIMA_APP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenopondo/Data Science/projects/clients/teal-insights/projects/p30-FIMA/FIMA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8198055E-8DC3-B14C-8628-F0E5FC92231A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378493F3-3802-D743-ADC1-DE9C4EABB919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
+    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="6" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
   </bookViews>
   <sheets>
     <sheet name="Macrofiscal" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Vulnerabilities" sheetId="4" r:id="rId4"/>
     <sheet name="Ratings" sheetId="5" r:id="rId5"/>
     <sheet name="Adjustment" sheetId="6" r:id="rId6"/>
+    <sheet name="About" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="89">
   <si>
     <t>Credit Rating</t>
   </si>
@@ -283,6 +284,30 @@
   </si>
   <si>
     <t>one_off_adjustment_to_debt_stock</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>prone_to</t>
+  </si>
+  <si>
+    <t>Ruritania is a tropical country whose main export is agricultural products. Before the pandemic the government was steadily making efforts consolidating the fiscal accounts which translated into a rating upgrade in 2021. The pandemic deteriorated the accounts and since then the government has been working to shore them up.</t>
+  </si>
+  <si>
+    <t>The country has been affected by droughts that have reduced its agricultural production. Heatwaves have decreased productivity and increased energy and water consumption. The country could benefit from better irrigation infrastructure and water management.</t>
+  </si>
+  <si>
+    <t>Aurelia is on the coast and has been affected by large hurricanes recently. With heavy rains there have been some serious landslides that have destroyed roads and other infrastructure. Climate scientist project that these events will increase in magnitude and frequency. The government is looking for financing to protect its growth and fiscal accounts from future events.</t>
+  </si>
+  <si>
+    <t>Rising sea levels have affected coastal towns and cities. Tourism is particularly vulnerable as beaches get narrower and infrastructure deteriorated. There are projects in place to improve protection for sea fronts and ports.</t>
+  </si>
+  <si>
+    <t>Xenon is a country that relies on labor-intensive manufacturing. The country has been affected by flooding due to unusually heavy rain. The government has built waterways and flood protection, but this has deteriorated its fiscal accounts in the process.</t>
+  </si>
+  <si>
+    <t>The government is interested in finding solutions that could improve its resilience to weather events without deteriorating its fiscal accounts. Borrowing cost increased after its credit rating fell from BB- to B+ in 2024.</t>
   </si>
 </sst>
 </file>
@@ -292,7 +317,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +335,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="3">
@@ -338,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -348,6 +378,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3204,7 +3235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1590C94F-F940-5443-969D-8E1E42D4E8F0}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -3529,4 +3560,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8305C3F5-26C6-544A-9B95-0DEC5FBA260B}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added country brief info
</commit_message>
<xml_diff>
--- a/data-raw/FIMA_APP.xlsx
+++ b/data-raw/FIMA_APP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenopondo/Data Science/projects/clients/teal-insights/projects/p30-FIMA/FIMA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378493F3-3802-D743-ADC1-DE9C4EABB919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A5A367-43F7-3D47-8F53-C5C0A17E0A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="6" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
+    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
   </bookViews>
   <sheets>
     <sheet name="Macrofiscal" sheetId="1" r:id="rId1"/>
@@ -2255,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849FA1A2-E33E-E344-A39E-F69BA8D5754B}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2446,7 +2446,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>53</v>
@@ -2457,7 +2457,7 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
@@ -2479,7 +2479,7 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>53</v>
@@ -2490,7 +2490,7 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>53</v>
@@ -2501,7 +2501,7 @@
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
         <v>53</v>
@@ -2512,7 +2512,7 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
@@ -2534,7 +2534,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>61</v>
@@ -2545,7 +2545,7 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
@@ -2556,7 +2556,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>61</v>
@@ -2578,7 +2578,7 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
         <v>61</v>
@@ -2600,7 +2600,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
         <v>61</v>
@@ -2611,7 +2611,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
         <v>53</v>
@@ -2622,7 +2622,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
         <v>53</v>
@@ -2633,7 +2633,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
         <v>53</v>
@@ -2644,7 +2644,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
         <v>53</v>
@@ -2655,7 +2655,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
         <v>53</v>
@@ -2666,7 +2666,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
@@ -2677,7 +2677,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
         <v>53</v>
@@ -2688,7 +2688,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
         <v>53</v>
@@ -2710,7 +2710,7 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
@@ -2721,7 +2721,7 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
@@ -2732,7 +2732,7 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
         <v>61</v>
@@ -2743,7 +2743,7 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
         <v>61</v>
@@ -2754,7 +2754,7 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>61</v>
@@ -2765,7 +2765,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
         <v>61</v>
@@ -2781,7 +2781,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2850,7 +2850,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2858,7 +2858,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2866,7 +2866,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2874,7 +2874,7 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2882,7 +2882,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2898,7 +2898,7 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2906,7 +2906,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3566,7 +3566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8305C3F5-26C6-544A-9B95-0DEC5FBA260B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added and improved contact panel
</commit_message>
<xml_diff>
--- a/data-raw/FIMA_APP.xlsx
+++ b/data-raw/FIMA_APP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenopondo/Data Science/projects/clients/teal-insights/projects/p30-FIMA/FIMA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A5A367-43F7-3D47-8F53-C5C0A17E0A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A6046D-A50F-EA4B-BD5E-3A162FE4A776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19900" activeTab="7" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
   </bookViews>
   <sheets>
     <sheet name="Macrofiscal" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Ratings" sheetId="5" r:id="rId5"/>
     <sheet name="Adjustment" sheetId="6" r:id="rId6"/>
     <sheet name="About" sheetId="7" r:id="rId7"/>
+    <sheet name="ColorCode" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="95">
   <si>
     <t>Credit Rating</t>
   </si>
@@ -308,6 +309,24 @@
   </si>
   <si>
     <t>The government is interested in finding solutions that could improve its resilience to weather events without deteriorating its fiscal accounts. Borrowing cost increased after its credit rating fell from BB- to B+ in 2024.</t>
+  </si>
+  <si>
+    <t>interventions</t>
+  </si>
+  <si>
+    <t>kpi</t>
+  </si>
+  <si>
+    <t>color_type</t>
+  </si>
+  <si>
+    <t>Dark green</t>
+  </si>
+  <si>
+    <t>Medium green</t>
+  </si>
+  <si>
+    <t>Light green</t>
   </si>
 </sst>
 </file>
@@ -342,7 +361,7 @@
       <name val="Aptos"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +371,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -379,6 +416,18 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2255,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849FA1A2-E33E-E344-A39E-F69BA8D5754B}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C46"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3619,4 +3668,668 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD58083-2AEE-6D4F-A687-DF21DEBA5EFA}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17">
+      <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17">
+      <c r="A4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17">
+      <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17">
+      <c r="A6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17">
+      <c r="A7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17">
+      <c r="A8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17">
+      <c r="A10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17">
+      <c r="A11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17">
+      <c r="A12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17">
+      <c r="A14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17">
+      <c r="A15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17">
+      <c r="A16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17">
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17">
+      <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17">
+      <c r="A19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17">
+      <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17">
+      <c r="A21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17">
+      <c r="A22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17">
+      <c r="A23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17">
+      <c r="A24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17">
+      <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17">
+      <c r="A26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17">
+      <c r="A27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17">
+      <c r="A28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17">
+      <c r="A29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17">
+      <c r="A31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17">
+      <c r="A32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17">
+      <c r="A33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17">
+      <c r="A34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17">
+      <c r="A35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17">
+      <c r="A36" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17">
+      <c r="A37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17">
+      <c r="A38" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17">
+      <c r="A39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17">
+      <c r="A40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17">
+      <c r="A41" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17">
+      <c r="A42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17">
+      <c r="A43" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17">
+      <c r="A44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17">
+      <c r="A45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17">
+      <c r="A46" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improved grammar of write up in home and documentation tab.
</commit_message>
<xml_diff>
--- a/data-raw/FIMA_APP.xlsx
+++ b/data-raw/FIMA_APP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reubenopondo/Data Science/projects/clients/teal-insights/projects/p30-FIMA/FIMA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A6046D-A50F-EA4B-BD5E-3A162FE4A776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA3272-E0B0-D14D-9F68-FDA5C8FEC781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19900" activeTab="7" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19900" activeTab="6" xr2:uid="{3951037A-9189-1849-A1DB-84DF4AE6714B}"/>
   </bookViews>
   <sheets>
     <sheet name="Macrofiscal" sheetId="1" r:id="rId1"/>
@@ -299,15 +299,9 @@
     <t>The country has been affected by droughts that have reduced its agricultural production. Heatwaves have decreased productivity and increased energy and water consumption. The country could benefit from better irrigation infrastructure and water management.</t>
   </si>
   <si>
-    <t>Aurelia is on the coast and has been affected by large hurricanes recently. With heavy rains there have been some serious landslides that have destroyed roads and other infrastructure. Climate scientist project that these events will increase in magnitude and frequency. The government is looking for financing to protect its growth and fiscal accounts from future events.</t>
-  </si>
-  <si>
     <t>Rising sea levels have affected coastal towns and cities. Tourism is particularly vulnerable as beaches get narrower and infrastructure deteriorated. There are projects in place to improve protection for sea fronts and ports.</t>
   </si>
   <si>
-    <t>Xenon is a country that relies on labor-intensive manufacturing. The country has been affected by flooding due to unusually heavy rain. The government has built waterways and flood protection, but this has deteriorated its fiscal accounts in the process.</t>
-  </si>
-  <si>
     <t>The government is interested in finding solutions that could improve its resilience to weather events without deteriorating its fiscal accounts. Borrowing cost increased after its credit rating fell from BB- to B+ in 2024.</t>
   </si>
   <si>
@@ -327,6 +321,12 @@
   </si>
   <si>
     <t>Light green</t>
+  </si>
+  <si>
+    <t>Aurelia has a long coast and has been affected by large hurricanes recently. Heavy rains have caused serious landslides that have destroyed roads and other infrastructure. Climate scientist project that these events will increase in magnitude and frequency. The government is looking for financial tools to protect its growth and fiscal accounts from future events.</t>
+  </si>
+  <si>
+    <t>Xenon is a country that relies on labor-intensive manufacturing. The country has been affected by flooding due to unusually heavy rain. The government has built waterways and flood barriers, but this has deteriorated its fiscal accounts.</t>
   </si>
 </sst>
 </file>
@@ -3615,8 +3615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8305C3F5-26C6-544A-9B95-0DEC5FBA260B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3637,10 +3637,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3659,10 +3659,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3674,7 +3674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD58083-2AEE-6D4F-A687-DF21DEBA5EFA}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -3687,16 +3687,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
@@ -3710,7 +3710,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -3724,7 +3724,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -3738,7 +3738,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -3752,7 +3752,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -3766,7 +3766,7 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -3780,7 +3780,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
@@ -3794,7 +3794,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
@@ -3808,7 +3808,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
@@ -3822,7 +3822,7 @@
         <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17">
@@ -3836,7 +3836,7 @@
         <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17">
@@ -3850,7 +3850,7 @@
         <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17">
@@ -3864,7 +3864,7 @@
         <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17">
@@ -3878,7 +3878,7 @@
         <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17">
@@ -3892,7 +3892,7 @@
         <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17">
@@ -3906,7 +3906,7 @@
         <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17">
@@ -3920,7 +3920,7 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17">
@@ -3934,7 +3934,7 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17">
@@ -3948,7 +3948,7 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17">
@@ -3962,7 +3962,7 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17">
@@ -3976,7 +3976,7 @@
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17">
@@ -3990,7 +3990,7 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17">
@@ -4004,7 +4004,7 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17">
@@ -4018,7 +4018,7 @@
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17">
@@ -4032,7 +4032,7 @@
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17">
@@ -4046,7 +4046,7 @@
         <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17">
@@ -4060,7 +4060,7 @@
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17">
@@ -4074,7 +4074,7 @@
         <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17">
@@ -4088,7 +4088,7 @@
         <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17">
@@ -4102,7 +4102,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17">
@@ -4116,7 +4116,7 @@
         <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17">
@@ -4130,7 +4130,7 @@
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17">
@@ -4144,7 +4144,7 @@
         <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17">
@@ -4158,7 +4158,7 @@
         <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17">
@@ -4172,7 +4172,7 @@
         <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17">
@@ -4186,7 +4186,7 @@
         <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17">
@@ -4200,7 +4200,7 @@
         <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17">
@@ -4214,7 +4214,7 @@
         <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17">
@@ -4228,7 +4228,7 @@
         <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17">
@@ -4242,7 +4242,7 @@
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17">
@@ -4256,7 +4256,7 @@
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17">
@@ -4270,7 +4270,7 @@
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17">
@@ -4284,7 +4284,7 @@
         <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17">
@@ -4298,7 +4298,7 @@
         <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17">
@@ -4312,7 +4312,7 @@
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17">
@@ -4326,7 +4326,7 @@
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>